<commit_message>
final changes for diss
</commit_message>
<xml_diff>
--- a/Results_round_1.xlsx
+++ b/Results_round_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Google Drive\UoL Computer Science\Level 3\Project\Round 1 Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\ml-covid19-eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D1552D-85B0-458F-8D5C-54071821A5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578D9C84-F7E0-463F-A8E7-263436C121E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -701,14 +701,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>

</xml_diff>